<commit_message>
1.0.3 Signed-off-by: HY-ZhengWei <HY.ZhengWei@qq.com>
</commit_message>
<xml_diff>
--- a/test/org/hy/common/report/junit/total/JU_Total_Subtotal.xlsx
+++ b/test/org/hy/common/report/junit/total/JU_Total_Subtotal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>人员名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,27 +45,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>入职时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:For:staffs.$size:staffs.$get(index).staffName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:For:staffs.$size:staffs.$get(index).time.YMD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分总人数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:staffs.$size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:For:staffs.$size:staffs.$get(index).staffNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>:orgName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>入职时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>:For:staffs.$size:staffs.$get(index).staffNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>:For:staffs.$size:staffs.$get(index).staffName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>:For:staffs.$size:staffs.$get(index).time.YMD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>部分总人数</t>
+    <t>小计：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -77,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,6 +110,24 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -117,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -177,11 +203,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -195,6 +311,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -204,11 +323,34 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,11 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -554,33 +696,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>11</v>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -588,27 +730,50 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:F5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
1.0.4 Signed-off-by: HY-ZhengWei <HY.ZhengWei@qq.com>
</commit_message>
<xml_diff>
--- a/test/org/hy/common/report/junit/total/JU_Total_Subtotal.xlsx
+++ b/test/org/hy/common/report/junit/total/JU_Total_Subtotal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>人员名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,14 @@
   </si>
   <si>
     <t>:staffMap[].time.YMD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合计：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:RowCount__</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -129,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +156,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -303,7 +317,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,6 +365,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -686,11 +724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:F5"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -771,11 +809,33 @@
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="18"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:F5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:F7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>